<commit_message>
Fix for 1900-1-1 date in datetime.date()
Issue #437.
</commit_message>
<xml_diff>
--- a/xlsxwriter/test/comparison/xlsx_files/date_1904_01.xlsx
+++ b/xlsxwriter/test/comparison/xlsx_files/date_1904_01.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -352,7 +352,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>